<commit_message>
Updated version with running imports
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="11_AD4DB114E441178AC67DF4273614C048683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C030475A-C160-40AD-84EA-51AA4464C66C}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="11_AD4DB114E441178AC67DF4273614C048683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77A2805D-7E2C-4F6F-9B41-D87CF16DF7DF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>ID</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t>Description 9</t>
+  </si>
+  <si>
+    <t>TransactionID</t>
   </si>
 </sst>
 </file>
@@ -507,7 +510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -675,7 +680,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -703,7 +708,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -778,19 +783,17 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A63201-BCAD-41F8-9FF2-8F5B41B5BB61}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="3" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -801,10 +804,13 @@
         <v>18</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -814,11 +820,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -830,11 +836,11 @@
       <c r="C3">
         <v>1</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:B7" si="0">A3+1</f>
         <v>3</v>
@@ -846,11 +852,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -862,11 +868,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -878,11 +884,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="E6" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -894,8 +900,22 @@
       <c r="C7">
         <v>1</v>
       </c>
-      <c r="D7" s="1">
+      <c r="E7" s="1">
         <v>0.01</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -908,7 +928,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFEB4EF-C391-4BFD-AEAC-515EF9165387}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -968,7 +988,7 @@
         <v>27</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1058,7 +1078,7 @@
         <v>37</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1094,7 +1114,7 @@
         <v>41</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some refactoring + Vote added
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="11_AD4DB114E441178AC67DF4273614C048683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{77A2805D-7E2C-4F6F-9B41-D87CF16DF7DF}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="11_AD4DB114E441178AC67DF4273614C048683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22CE15D3-A36E-4988-B799-28D1E5138216}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
-    <sheet name="Wallets" sheetId="3" r:id="rId3"/>
-    <sheet name="WalletTransactions" sheetId="4" r:id="rId4"/>
-    <sheet name="Issues" sheetId="5" r:id="rId5"/>
+    <sheet name="Issues" sheetId="5" r:id="rId3"/>
+    <sheet name="Suggestions" sheetId="6" r:id="rId4"/>
+    <sheet name="StakedSuggestions" sheetId="7" r:id="rId5"/>
+    <sheet name="Wallets" sheetId="3" r:id="rId6"/>
+    <sheet name="WalletTransactions" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>ID</t>
   </si>
@@ -167,6 +169,21 @@
   </si>
   <si>
     <t>TransactionID</t>
+  </si>
+  <si>
+    <t>IssueID</t>
+  </si>
+  <si>
+    <t>Issue 1 Suggestion 1</t>
+  </si>
+  <si>
+    <t>Suggestion 1</t>
+  </si>
+  <si>
+    <t>Suggestion 2</t>
+  </si>
+  <si>
+    <t>SuggestionID</t>
   </si>
 </sst>
 </file>
@@ -216,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -228,6 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -510,9 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -676,6 +692,295 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFEB4EF-C391-4BFD-AEAC-515EF9165387}">
+  <dimension ref="A1:E10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" customWidth="1"/>
+    <col min="4" max="4" width="21.5703125" customWidth="1"/>
+    <col min="5" max="5" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="str">
+        <f>CONCATENATE("#tag",TEXT(A2,"0"),".1 #tag",TEXT(A2,"0"),".2 #tag",TEXT(A2,"0"),".3")</f>
+        <v>#tag1.1 #tag1.2 #tag1.3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B10" si="0">CONCATENATE("#tag",TEXT(A3,"0"),".1 #tag",TEXT(A3,"0"),".2 #tag",TEXT(A3,"0"),".3")</f>
+        <v>#tag2.1 #tag2.2 #tag2.3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" si="0"/>
+        <v>#tag3.1 #tag3.2 #tag3.3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>#tag4.1 #tag4.2 #tag4.3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>#tag5.1 #tag5.2 #tag5.3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>#tag6.1 #tag6.2 #tag6.3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>#tag7.1 #tag7.2 #tag7.3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>#tag8.1 #tag8.2 #tag8.3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>#tag9.1 #tag9.2 #tag9.3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAD70F6-15E6-4154-ACD5-2D878890659E}">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="28.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F944EBF-513D-4822-9A80-D94BD1F4FC73}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C81D79-5771-4AF5-893D-311099C14369}">
   <dimension ref="A1:C7"/>
   <sheetViews>
@@ -781,7 +1086,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A63201-BCAD-41F8-9FF2-8F5B41B5BB61}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -914,6 +1219,9 @@
       <c r="C8">
         <v>4</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
       <c r="E8" s="1">
         <v>99</v>
       </c>
@@ -922,203 +1230,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFEB4EF-C391-4BFD-AEAC-515EF9165387}">
-  <dimension ref="A1:E10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" customWidth="1"/>
-    <col min="4" max="4" width="21.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="str">
-        <f>CONCATENATE("#tag",TEXT(A2,"0"),".1 #tag",TEXT(A2,"0"),".2 #tag",TEXT(A2,"0"),".3")</f>
-        <v>#tag1.1 #tag1.2 #tag1.3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="str">
-        <f t="shared" ref="B3:B10" si="0">CONCATENATE("#tag",TEXT(A3,"0"),".1 #tag",TEXT(A3,"0"),".2 #tag",TEXT(A3,"0"),".3")</f>
-        <v>#tag2.1 #tag2.2 #tag2.3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="str">
-        <f t="shared" si="0"/>
-        <v>#tag3.1 #tag3.2 #tag3.3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="str">
-        <f t="shared" si="0"/>
-        <v>#tag4.1 #tag4.2 #tag4.3</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="str">
-        <f t="shared" si="0"/>
-        <v>#tag5.1 #tag5.2 #tag5.3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="str">
-        <f t="shared" si="0"/>
-        <v>#tag6.1 #tag6.2 #tag6.3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="str">
-        <f t="shared" si="0"/>
-        <v>#tag7.1 #tag7.2 #tag7.3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>36</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="str">
-        <f t="shared" si="0"/>
-        <v>#tag8.1 #tag8.2 #tag8.3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
-      </c>
-      <c r="E9">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="str">
-        <f t="shared" si="0"/>
-        <v>#tag9.1 #tag9.2 #tag9.3</v>
-      </c>
-      <c r="C10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added basic webservice and blazer app with authentication
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="11_AD4DB114E441178AC67DF4273614C048683EDF18" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{22CE15D3-A36E-4988-B799-28D1E5138216}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{01CE5C2D-36AC-430A-AAD5-A4C483CB7B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2D0570D-9D80-421F-B63B-6F42FBA51450}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
   <si>
     <t>ID</t>
   </si>
@@ -184,6 +184,15 @@
   </si>
   <si>
     <t>SuggestionID</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>UniqueExternalUserID</t>
+  </si>
+  <si>
+    <t>5f5a978a-4595-4e07-b456-73bf26fe6786</t>
   </si>
 </sst>
 </file>
@@ -233,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -246,6 +255,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -615,26 +625,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1141671-137E-4736-8FCB-A2722CE9603E}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -642,7 +654,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -651,7 +663,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A6" si="0">A3+1</f>
         <v>3</v>
@@ -660,7 +672,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -669,7 +681,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -677,13 +689,24 @@
       <c r="B6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -982,11 +1005,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72C81D79-5771-4AF5-893D-311099C14369}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1081,6 +1102,17 @@
         <v>0.01</v>
       </c>
     </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1088,9 +1120,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8A63201-BCAD-41F8-9FF2-8F5B41B5BB61}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1226,6 +1258,20 @@
         <v>99</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update with rules for issues implemented
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{01CE5C2D-36AC-430A-AAD5-A4C483CB7B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2D0570D-9D80-421F-B63B-6F42FBA51450}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{01CE5C2D-36AC-430A-AAD5-A4C483CB7B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26C1B1B8-4B64-4148-A94F-2C1C8480166F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>5f5a978a-4595-4e07-b456-73bf26fe6786</t>
+  </si>
+  <si>
+    <t>CreatorUserID</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1141671-137E-4736-8FCB-A2722CE9603E}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -716,9 +719,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFEB4EF-C391-4BFD-AEAC-515EF9165387}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -726,9 +731,10 @@
     <col min="3" max="3" width="14.5703125" customWidth="1"/>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -744,8 +750,11 @@
       <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -762,8 +771,11 @@
       <c r="E2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -777,8 +789,11 @@
       <c r="D3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -792,8 +807,11 @@
       <c r="D4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -807,8 +825,11 @@
       <c r="D5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -822,8 +843,11 @@
       <c r="D6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -837,8 +861,11 @@
       <c r="D7" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -855,8 +882,11 @@
       <c r="E8">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -873,8 +903,11 @@
       <c r="E9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -890,6 +923,9 @@
       </c>
       <c r="E10">
         <v>10</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some fixes + wallet controller added
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{01CE5C2D-36AC-430A-AAD5-A4C483CB7B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26C1B1B8-4B64-4148-A94F-2C1C8480166F}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{01CE5C2D-36AC-430A-AAD5-A4C483CB7B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F64A775-6AE6-4AE9-9E0B-E80572255FBA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -721,7 +721,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFEB4EF-C391-4BFD-AEAC-515EF9165387}">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -936,17 +936,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DAD70F6-15E6-4154-ACD5-2D878890659E}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="28.7109375" customWidth="1"/>
     <col min="4" max="4" width="21.42578125" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -959,8 +960,11 @@
       <c r="D1" s="5" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -973,8 +977,11 @@
       <c r="D2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -986,6 +993,9 @@
       </c>
       <c r="D3" t="s">
         <v>46</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed old Blazor App, Added Voting
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5EEE666D-0E05-4FCD-900D-7D9A1B62D716}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5F56F3B-E3A5-456A-A780-74C85AD517AD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -314,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -329,6 +329,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -647,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -832,7 +838,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F1" sqref="F1:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -930,6 +936,9 @@
       <c r="D5" t="s">
         <v>34</v>
       </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
       <c r="F5">
         <v>4</v>
       </c>
@@ -959,22 +968,21 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5703125" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" customWidth="1"/>
-    <col min="5" max="1025" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="153" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="1025" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -984,11 +992,14 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1001,8 +1012,11 @@
       <c r="D2" s="7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1012,11 +1026,14 @@
       <c r="C3" t="s">
         <v>41</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="9" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1026,11 +1043,14 @@
       <c r="C4" t="s">
         <v>43</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="9" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1040,11 +1060,14 @@
       <c r="C5" t="s">
         <v>45</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1054,11 +1077,14 @@
       <c r="C6" t="s">
         <v>47</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="9" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1068,11 +1094,14 @@
       <c r="C7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="9" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1082,11 +1111,14 @@
       <c r="C8" t="s">
         <v>51</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="9" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1096,11 +1128,14 @@
       <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="9" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1110,11 +1145,14 @@
       <c r="C10" t="s">
         <v>55</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1124,11 +1162,14 @@
       <c r="C11" t="s">
         <v>57</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="9" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1138,11 +1179,14 @@
       <c r="C12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="9" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1152,11 +1196,14 @@
       <c r="C13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="9" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1166,11 +1213,14 @@
       <c r="C14" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="9" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1180,8 +1230,11 @@
       <c r="C15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1191,11 +1244,14 @@
       <c r="C16" t="s">
         <v>66</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="9" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1205,13 +1261,16 @@
       <c r="C17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="9" t="s">
         <v>69</v>
+      </c>
+      <c r="E17">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1219,7 +1278,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Web-Assembly with OIC Authentification added
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F5F56F3B-E3A5-456A-A780-74C85AD517AD}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F6184C0-AEC8-4040-916A-21E0DDADE919}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -87,9 +87,6 @@
     <t>Andreas</t>
   </si>
   <si>
-    <t>5f5a978a-4595-4e07-b456-73bf26fe6786</t>
-  </si>
-  <si>
     <t>NoBalance</t>
   </si>
   <si>
@@ -271,6 +268,9 @@
   </si>
   <si>
     <t>Balance</t>
+  </si>
+  <si>
+    <t>99151f7e-ea87-47bb-8556-3401c7ba87c2</t>
   </si>
 </sst>
 </file>
@@ -653,7 +653,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -743,7 +743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -808,7 +808,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>15</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -816,7 +816,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -824,7 +824,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -857,19 +857,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -877,13 +877,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
         <v>23</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -894,13 +894,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -911,13 +911,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
         <v>29</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>30</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -928,13 +928,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>33</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -948,13 +948,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
         <v>35</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>36</v>
-      </c>
-      <c r="D6" t="s">
-        <v>37</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -987,16 +987,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="8" t="s">
-        <v>20</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1007,10 +1007,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>39</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>40</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1024,10 +1024,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="9" t="s">
         <v>41</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>42</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -1041,10 +1041,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>43</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1058,10 +1058,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>45</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>46</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1075,10 +1075,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="9" t="s">
         <v>47</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>48</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1092,10 +1092,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="9" t="s">
         <v>49</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>50</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1109,10 +1109,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>51</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>52</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1126,10 +1126,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1143,10 +1143,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>55</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1160,10 +1160,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>57</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>58</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1177,10 +1177,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="D12" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1194,10 +1194,10 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="9" t="s">
         <v>61</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>62</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1211,10 +1211,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="9" t="s">
         <v>63</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>64</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1228,7 +1228,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -1242,10 +1242,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1259,10 +1259,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>68</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>69</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1292,13 +1292,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>71</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1340,10 +1340,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>71</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1458,16 +1458,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Renamed suggestions into proposal
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="42" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3EA1221-6E27-46BA-8232-3741F1028433}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F101760-61B6-4163-A62C-E616F6CCE13E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="22320" windowHeight="13560" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
     <sheet name="Users" sheetId="2" r:id="rId2"/>
     <sheet name="Issues" sheetId="3" r:id="rId3"/>
-    <sheet name="Suggestions" sheetId="4" r:id="rId4"/>
-    <sheet name="StakedSuggestions" sheetId="5" r:id="rId5"/>
+    <sheet name="Proposals" sheetId="4" r:id="rId4"/>
+    <sheet name="StakedProposals" sheetId="5" r:id="rId5"/>
     <sheet name="Wallets" sheetId="6" r:id="rId6"/>
     <sheet name="WalletTransactions" sheetId="7" r:id="rId7"/>
   </sheets>
@@ -57,15 +57,6 @@
     <t>AddIssue</t>
   </si>
   <si>
-    <t>AddSuggestion</t>
-  </si>
-  <si>
-    <t>StakeSuggestion</t>
-  </si>
-  <si>
-    <t>StakeSuggestionRollback</t>
-  </si>
-  <si>
     <t>UserName</t>
   </si>
   <si>
@@ -249,9 +240,6 @@
     <t>Alle Gesetze sollen künftig mit einer CO2-Bremse auf ihre Klimawirkung hin überprüft werden. Außerdem möchte die Partei ein Klimaschutz-Sofortprogramm auflegen, das Klimaschutzgesetz nachschärfen, Kohleausstieg bereits bis 2030 statt bis 2038 vollziehen.</t>
   </si>
   <si>
-    <t>SuggestionID</t>
-  </si>
-  <si>
     <t>UserID</t>
   </si>
   <si>
@@ -274,6 +262,18 @@
   </si>
   <si>
     <t>a76bb607-c937-49f0-a6ad-06c0a2398fd7</t>
+  </si>
+  <si>
+    <t>AddProposal</t>
+  </si>
+  <si>
+    <t>StakeProposal</t>
+  </si>
+  <si>
+    <t>StakeProposalRollback</t>
+  </si>
+  <si>
+    <t>ProposalID</t>
   </si>
 </sst>
 </file>
@@ -656,7 +656,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -706,7 +708,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="C4" s="2">
         <v>-3</v>
@@ -718,7 +720,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>75</v>
       </c>
       <c r="C5" s="2">
         <v>-1</v>
@@ -730,7 +732,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>76</v>
       </c>
       <c r="C6" s="2">
         <v>1</v>
@@ -746,7 +748,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -761,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,7 +774,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -781,7 +783,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -790,7 +792,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -799,7 +801,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -808,10 +810,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -819,7 +821,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -827,7 +829,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -835,7 +837,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -868,19 +870,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -888,13 +890,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F2">
         <v>5</v>
@@ -905,13 +907,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -922,13 +924,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4">
         <v>4</v>
@@ -939,13 +941,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>100</v>
@@ -959,13 +961,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -998,16 +1000,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1018,10 +1020,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -1035,10 +1037,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -1052,10 +1054,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -1069,10 +1071,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1086,10 +1088,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1103,10 +1105,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1120,10 +1122,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1137,10 +1139,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -1154,10 +1156,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -1171,10 +1173,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -1188,10 +1190,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -1205,10 +1207,10 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -1222,10 +1224,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -1239,7 +1241,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -1253,10 +1255,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -1270,10 +1272,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -1303,13 +1305,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1351,10 +1353,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1480,16 +1482,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Image + updated Excel sheet
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="49" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{63EC885D-A60D-43F3-82F6-F94EC6026141}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="11_008D8CD54122C760501209B013968A9A81669F88" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{83635D5B-1C55-446B-A7A3-D417A23B6E23}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="StakedProposals" sheetId="5" r:id="rId5"/>
     <sheet name="Wallets" sheetId="6" r:id="rId6"/>
     <sheet name="WalletTransactions" sheetId="7" r:id="rId7"/>
+    <sheet name="Images" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
   <si>
     <t>ID</t>
   </si>
@@ -274,13 +275,22 @@
   </si>
   <si>
     <t>#Klima #CO2 #Umweltschutz</t>
+  </si>
+  <si>
+    <t>Hashtags</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>windmills-5643293_1280.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -295,6 +305,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -317,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -340,6 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -850,8 +868,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1637,4 +1655,38 @@
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCFA348-F033-495C-BB31-4195C34575EB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
+    <col min="2" max="2" width="37.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Minor updates for docker handling and presentations
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_1C8BC1380481439A2AEB65CB8DC1830C3A7E695F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_1C8BC1380481439A2AEB65CB8DC1830C3A7E695F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{961828E2-C7DD-4F1D-9A2A-798FFAC63D2A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="349">
   <si>
     <t>ID</t>
   </si>
@@ -958,9 +958,6 @@
   </si>
   <si>
     <t>default</t>
-  </si>
-  <si>
-    <t>windmills-5643293_1280.jpg</t>
   </si>
   <si>
     <t>welding.jpg</t>
@@ -1677,7 +1674,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3751,10 +3748,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:B84"/>
+  <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3779,7 +3776,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>302</v>
@@ -3787,7 +3784,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
         <v>303</v>
@@ -3795,7 +3792,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>304</v>
@@ -3803,7 +3800,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B6" t="s">
         <v>305</v>
@@ -3811,23 +3808,23 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
+    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>39</v>
       </c>
       <c r="B8" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
-        <v>39</v>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>42</v>
       </c>
       <c r="B9" t="s">
         <v>308</v>
@@ -3835,7 +3832,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
         <v>309</v>
@@ -3843,7 +3840,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
         <v>310</v>
@@ -3851,7 +3848,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>311</v>
@@ -3859,23 +3856,23 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B13" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>54</v>
+    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>313</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
-        <v>57</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
       </c>
       <c r="B15" t="s">
         <v>314</v>
@@ -3883,55 +3880,55 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B16" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>63</v>
+    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="B17" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B18" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>69</v>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>72</v>
       </c>
       <c r="B19" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>72</v>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>75</v>
       </c>
       <c r="B20" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>75</v>
-      </c>
-      <c r="B21" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="8" t="s">
-        <v>78</v>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
       </c>
       <c r="B22" t="s">
         <v>319</v>
@@ -3939,7 +3936,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
         <v>320</v>
@@ -3947,7 +3944,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B24" t="s">
         <v>321</v>
@@ -3955,7 +3952,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B25" t="s">
         <v>322</v>
@@ -3963,7 +3960,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B26" t="s">
         <v>323</v>
@@ -3971,7 +3968,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
         <v>324</v>
@@ -3979,7 +3976,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B28" t="s">
         <v>325</v>
@@ -3987,7 +3984,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B29" t="s">
         <v>326</v>
@@ -3995,7 +3992,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B30" t="s">
         <v>327</v>
@@ -4003,7 +4000,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="B31" t="s">
         <v>328</v>
@@ -4011,7 +4008,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="B32" t="s">
         <v>329</v>
@@ -4019,23 +4016,23 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="B33" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>114</v>
-      </c>
       <c r="B34" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="8" t="s">
         <v>331</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>120</v>
       </c>
       <c r="B35" t="s">
         <v>332</v>
@@ -4043,7 +4040,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="B36" t="s">
         <v>333</v>
@@ -4051,55 +4048,55 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="B37" t="s">
-        <v>334</v>
+        <v>312</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="B38" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="B39" t="s">
-        <v>308</v>
+        <v>334</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B40" t="s">
-        <v>335</v>
+        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="B41" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B42" t="s">
-        <v>310</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B43" t="s">
         <v>336</v>
@@ -4107,151 +4104,151 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B44" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B45" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B46" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>153</v>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>156</v>
       </c>
       <c r="B47" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
-        <v>156</v>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>159</v>
       </c>
       <c r="B48" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="B49" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>162</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>24</v>
+        <v>167</v>
       </c>
       <c r="B51" t="s">
-        <v>313</v>
+        <v>337</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B52" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B53" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B54" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B55" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B56" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B57" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>185</v>
+        <v>111</v>
       </c>
       <c r="B58" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>111</v>
+        <v>190</v>
       </c>
       <c r="B59" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>190</v>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>193</v>
       </c>
       <c r="B60" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="B61" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="8" t="s">
-        <v>196</v>
+        <v>339</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>199</v>
       </c>
       <c r="B62" t="s">
         <v>340</v>
@@ -4259,7 +4256,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="B63" t="s">
         <v>341</v>
@@ -4267,95 +4264,95 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B64" t="s">
-        <v>342</v>
+        <v>314</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>205</v>
+        <v>123</v>
       </c>
       <c r="B65" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>123</v>
+        <v>209</v>
       </c>
       <c r="B66" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>209</v>
+        <v>322</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" s="8" t="s">
+        <v>212</v>
       </c>
       <c r="B67" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="8" t="s">
-        <v>212</v>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>215</v>
       </c>
       <c r="B68" t="s">
-        <v>338</v>
+        <v>314</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B69" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B70" t="s">
-        <v>323</v>
+        <v>342</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B71" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>224</v>
+        <v>84</v>
       </c>
       <c r="B72" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>84</v>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>227</v>
       </c>
       <c r="B73" t="s">
-        <v>321</v>
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="B74" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
-        <v>230</v>
+        <v>343</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>233</v>
       </c>
       <c r="B75" t="s">
         <v>344</v>
@@ -4363,7 +4360,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="B76" t="s">
         <v>345</v>
@@ -4371,31 +4368,31 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="B77" t="s">
-        <v>346</v>
+        <v>310</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="B78" t="s">
-        <v>311</v>
+        <v>337</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="B79" t="s">
-        <v>338</v>
+        <v>346</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="B80" t="s">
         <v>347</v>
@@ -4403,34 +4400,26 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="B81" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="B82" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B83" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>257</v>
-      </c>
-      <c r="B84" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added image preview on browsing of existing hashtags
</commit_message>
<xml_diff>
--- a/Frontend/TestConsole/TestData.xlsx
+++ b/Frontend/TestConsole/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/182ce14098f0e49b/Dokumente/pnyx/Frontend/TestConsole/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_1C8BC1380481439A2AEB65CB8DC1830C3A7E695F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{961828E2-C7DD-4F1D-9A2A-798FFAC63D2A}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="11_1C8BC1380481439A2AEB65CB8DC1830C3A7E695F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3EC72849-4837-4BF4-B99D-070AC33D2D7C}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TransactionTypes" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="350">
   <si>
     <t>ID</t>
   </si>
@@ -160,10 +160,6 @@
     <t>Kann der Staat das Klima schützen und wenn ja wie?</t>
   </si>
   <si>
-    <t xml:space="preserve">#bundeswehr #militär #innenpolitik #terrorismusbekämpfung 
-#bundeswehr #inlandeinsatz </t>
-  </si>
-  <si>
     <t>Bundeswehr im Inneren</t>
   </si>
   <si>
@@ -215,10 +211,6 @@
     <t>BAföG soll generell unabhängig vom Einkommen der Eltern gezahlt werden.</t>
   </si>
   <si>
-    <t>#videoüberwachung #ausweitungvideoüberwachung 
-#überwachung</t>
-  </si>
-  <si>
     <t>Ausweitung der Videoüberwachung</t>
   </si>
   <si>
@@ -243,10 +235,6 @@
     <t>Generelles Tempolimit auf Autobahnen!</t>
   </si>
   <si>
-    <t>#verteidigungsausgaben #verteidigung #verteidigungspolitik
-#rüstungspolitik #rüstung</t>
-  </si>
-  <si>
     <t>Erhöhung der Verteidigungsausgaben</t>
   </si>
   <si>
@@ -262,10 +250,6 @@
     <t>Betreiber von Internetseiten sollen gesetzlich dazu verpflichtet sein, Falschinformationen ("Fake News") zu löschen, auf die sie hingewiesen wurden.</t>
   </si>
   <si>
-    <t>#ökologischelandwirtschaft #landwirtschaft #öko 
-#konventionellelandwirtschaft</t>
-  </si>
-  <si>
     <t>Ökologische Landwirtschaft</t>
   </si>
   <si>
@@ -281,10 +265,6 @@
     <t>Kindergeld soll nur an deutsche Familien ausgezahlt werden.</t>
   </si>
   <si>
-    <t>#befristung #sachgrundlosebefristung #arbeitsverträge
-#befristetearbeitsverträge</t>
-  </si>
-  <si>
     <t>Sachgrundlose Befristung</t>
   </si>
   <si>
@@ -516,10 +496,6 @@
     <t>Deutschland soll den Euro als Währung behalten.</t>
   </si>
   <si>
-    <t>#europa #eu #bürgerentscheide #direktedemokratie
-#bürgerinitiativen</t>
-  </si>
-  <si>
     <t>EU-weite Bürgerentscheide</t>
   </si>
   <si>
@@ -628,20 +604,12 @@
     <t>Die EU-Mitgliedsstaaten sollen eine gemeinsame Armee schaffen.</t>
   </si>
   <si>
-    <t>#kommissionspräsidentin #europäischekommision 
-#europäischeunion</t>
-  </si>
-  <si>
     <t>Direktwahl des Kommissionspräsidenten</t>
   </si>
   <si>
     <t>Der Präsident der Europäischen Kommission soll von den Bürgerinnen und Bürgern der Europäischen Union direkt gewählt werden.</t>
   </si>
   <si>
-    <t>#gleichgeschlechtlicheehen #europäischeunion #ehe 
-#mitgliedsstaaten</t>
-  </si>
-  <si>
     <t>Gleichgeschlechtliche Ehen</t>
   </si>
   <si>
@@ -687,10 +655,6 @@
     <t>Alle Staaten der Eurozone sollen für die Kreditaufnahme der anderen Staaten haften können.</t>
   </si>
   <si>
-    <t>#berufsabschluss #anerkennungberufsabschluss #eu
-#europäischeunion</t>
-  </si>
-  <si>
     <t>Anerkennung von Berufsabschlüssen</t>
   </si>
   <si>
@@ -733,20 +697,12 @@
     <t>Die gemeinsame Außenpolitik der Europäischen Union soll ausgebaut werden.</t>
   </si>
   <si>
-    <t>#asyl #asylsuchende #obergrenze #asylsuchende 
-#europäischeunion</t>
-  </si>
-  <si>
     <t>Asylgesetze</t>
   </si>
   <si>
     <t>In allen Ländern der Europäischen Union sollen gleiche Regeln für die Aufnahme von Asylsuchenden gelten.</t>
   </si>
   <si>
-    <t>#volksentscheide #direktedemokratie #eu
-#europäischeunion</t>
-  </si>
-  <si>
     <t>Volksentscheide über EU-Vertragsänderungen</t>
   </si>
   <si>
@@ -1044,10 +1000,6 @@
     <t>frauenquote.jpg</t>
   </si>
   <si>
-    <t>#verurteilungminderjähriger #verurteilung #kinderverurteilung
-#minderjährige</t>
-  </si>
-  <si>
     <t>kids.jpg</t>
   </si>
   <si>
@@ -1100,6 +1052,45 @@
   </si>
   <si>
     <t>bussi.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#bundeswehr #militär #innenpolitik #terrorismusbekämpfung #inlandeinsatz </t>
+  </si>
+  <si>
+    <t>#verteidigungsausgaben #verteidigung #verteidigungspolitik #rüstungspolitik #rüstung</t>
+  </si>
+  <si>
+    <t>#ökologischelandwirtschaft #landwirtschaft #öko #konventionellelandwirtschaft</t>
+  </si>
+  <si>
+    <t>#befristung #sachgrundlosebefristung #arbeitsverträge #befristetearbeitsverträge</t>
+  </si>
+  <si>
+    <t>#verurteilungminderjähriger #verurteilung #kinderverurteilung #minderjährige</t>
+  </si>
+  <si>
+    <t>#europa #eu #bürgerentscheide #direktedemokratie #bürgerinitiativen</t>
+  </si>
+  <si>
+    <t>#kommissionspräsidentin #europäischekommision #europäischeunion</t>
+  </si>
+  <si>
+    <t>#gleichgeschlechtlicheehen #europäischeunion #ehe #mitgliedsstaaten</t>
+  </si>
+  <si>
+    <t>#berufsabschluss #anerkennungberufsabschluss #eu #europäischeunion</t>
+  </si>
+  <si>
+    <t>#asyl #asylsuchende #obergrenze #asylsuchende #europäischeunion</t>
+  </si>
+  <si>
+    <t>#volksentscheide #direktedemokratie #eu #europäischeunion</t>
+  </si>
+  <si>
+    <t>#videoüberwachung #ausweitungvideoüberwachung #überwachung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#bundeswehr #militär #innenpolitik #terrorismusbekämpfung #bundeswehr #inlandeinsatz </t>
   </si>
 </sst>
 </file>
@@ -1574,7 +1565,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView zoomScale="200" zoomScaleNormal="200" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1674,9 +1667,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F82"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
+    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1795,18 +1786,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="C7" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>41</v>
       </c>
       <c r="F7">
         <v>5</v>
@@ -1817,13 +1808,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="F8">
         <v>5</v>
@@ -1834,13 +1825,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
         <v>45</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="F9">
         <v>5</v>
@@ -1851,13 +1842,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
         <v>48</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>50</v>
       </c>
       <c r="F10">
         <v>5</v>
@@ -1868,13 +1859,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" t="s">
         <v>51</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>53</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -1885,13 +1876,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
         <v>54</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>56</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -1902,13 +1893,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="C13" t="s">
-        <v>58</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -1919,13 +1910,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="F14">
         <v>5</v>
@@ -1936,30 +1927,30 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" t="s">
+        <v>62</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>65</v>
-      </c>
       <c r="F15">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>66</v>
+        <v>338</v>
       </c>
       <c r="C16" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F16">
         <v>5</v>
@@ -1970,13 +1961,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F17">
         <v>5</v>
@@ -1987,13 +1978,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>72</v>
+        <v>339</v>
       </c>
       <c r="C18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F18">
         <v>5</v>
@@ -2004,13 +1995,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F19">
         <v>5</v>
@@ -2021,13 +2012,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>78</v>
+        <v>340</v>
       </c>
       <c r="C20" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="F20">
         <v>5</v>
@@ -2038,13 +2029,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="F21">
         <v>5</v>
@@ -2055,13 +2046,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F22">
         <v>5</v>
@@ -2072,13 +2063,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="F23">
         <v>5</v>
@@ -2089,13 +2080,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F24">
         <v>5</v>
@@ -2106,13 +2097,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C25" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F25">
         <v>5</v>
@@ -2123,13 +2114,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C26" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F26">
         <v>5</v>
@@ -2140,13 +2131,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D27" s="6" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F27">
         <v>5</v>
@@ -2157,13 +2148,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C28" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="F28">
         <v>5</v>
@@ -2174,13 +2165,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F29">
         <v>5</v>
@@ -2191,13 +2182,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C30" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="F30">
         <v>5</v>
@@ -2208,13 +2199,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F31">
         <v>5</v>
@@ -2225,13 +2216,13 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C32" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="D32" s="6" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F32">
         <v>5</v>
@@ -2242,13 +2233,13 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C33" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F33">
         <v>5</v>
@@ -2259,13 +2250,13 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C34" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F34">
         <v>5</v>
@@ -2276,13 +2267,13 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F35">
         <v>5</v>
@@ -2293,13 +2284,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C36" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F36">
         <v>5</v>
@@ -2310,13 +2301,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C37" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F37">
         <v>5</v>
@@ -2327,13 +2318,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C38" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F38">
         <v>5</v>
@@ -2344,13 +2335,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C39" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F39">
         <v>5</v>
@@ -2361,13 +2352,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D40" s="6" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F40">
         <v>5</v>
@@ -2378,13 +2369,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C41" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F41">
         <v>5</v>
@@ -2395,13 +2386,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C42" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F42">
         <v>5</v>
@@ -2412,13 +2403,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F43">
         <v>5</v>
@@ -2429,13 +2420,13 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C44" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="F44">
         <v>5</v>
@@ -2446,13 +2437,13 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C45" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F45">
         <v>5</v>
@@ -2463,13 +2454,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>156</v>
+        <v>342</v>
       </c>
       <c r="C46" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D46" s="6" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F46">
         <v>5</v>
@@ -2480,13 +2471,13 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="C47" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="F47">
         <v>5</v>
@@ -2497,13 +2488,13 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="C48" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D48" s="6" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F48">
         <v>5</v>
@@ -2517,10 +2508,10 @@
         <v>24</v>
       </c>
       <c r="C49" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="F49">
         <v>5</v>
@@ -2531,13 +2522,13 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="C50" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D50" s="6" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F50">
         <v>5</v>
@@ -2548,13 +2539,13 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="F51">
         <v>5</v>
@@ -2565,13 +2556,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="C52" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D52" s="6" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="F52">
         <v>5</v>
@@ -2582,13 +2573,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="C53" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D53" s="6" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F53">
         <v>5</v>
@@ -2599,13 +2590,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="C54" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="D54" s="6" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F54">
         <v>5</v>
@@ -2616,13 +2607,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D55" s="6" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="F55">
         <v>5</v>
@@ -2633,13 +2624,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="C56" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F56">
         <v>5</v>
@@ -2650,13 +2641,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C57" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="F57">
         <v>5</v>
@@ -2667,13 +2658,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C58" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D58" s="6" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F58">
         <v>5</v>
@@ -2684,13 +2675,13 @@
         <v>58</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>193</v>
+        <v>343</v>
       </c>
       <c r="C59" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="F59">
         <v>5</v>
@@ -2701,13 +2692,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>196</v>
+        <v>344</v>
       </c>
       <c r="C60" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D60" s="6" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F60">
         <v>5</v>
@@ -2718,13 +2709,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C61" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="F61">
         <v>5</v>
@@ -2735,13 +2726,13 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C62" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="F62">
         <v>5</v>
@@ -2752,13 +2743,13 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C63" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
       <c r="F63">
         <v>5</v>
@@ -2769,13 +2760,13 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C64" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="F64">
         <v>5</v>
@@ -2786,13 +2777,13 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="C65" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
       <c r="F65">
         <v>5</v>
@@ -2803,13 +2794,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>212</v>
+        <v>345</v>
       </c>
       <c r="C66" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="F66">
         <v>5</v>
@@ -2820,13 +2811,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C67" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="F67">
         <v>5</v>
@@ -2837,13 +2828,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="C68" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="F68">
         <v>5</v>
@@ -2854,13 +2845,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C69" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F69">
         <v>5</v>
@@ -2871,13 +2862,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="C70" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="F70">
         <v>5</v>
@@ -2888,13 +2879,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C71" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F71">
         <v>5</v>
@@ -2905,13 +2896,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>227</v>
+        <v>346</v>
       </c>
       <c r="C72" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D72" s="6" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="F72">
         <v>5</v>
@@ -2922,13 +2913,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>230</v>
+        <v>347</v>
       </c>
       <c r="C73" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="D73" s="6" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="F73">
         <v>5</v>
@@ -2939,13 +2930,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="C74" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F74">
         <v>5</v>
@@ -2956,13 +2947,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="C75" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="F75">
         <v>5</v>
@@ -2973,13 +2964,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="C76" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="F76">
         <v>5</v>
@@ -2990,13 +2981,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="C77" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="F77">
         <v>5</v>
@@ -3007,13 +2998,13 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="C78" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="F78">
         <v>5</v>
@@ -3024,13 +3015,13 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="C79" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="F79">
         <v>5</v>
@@ -3041,13 +3032,13 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C80" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="F80">
         <v>5</v>
@@ -3058,13 +3049,13 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="C81" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="D81" s="6" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="F81">
         <v>5</v>
@@ -3075,13 +3066,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C82" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="D82" s="6" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="F82">
         <v>5</v>
@@ -3112,7 +3103,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="C1" s="9" t="s">
         <v>20</v>
@@ -3132,10 +3123,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -3149,10 +3140,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -3166,10 +3157,10 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="E4">
         <v>4</v>
@@ -3183,10 +3174,10 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -3200,10 +3191,10 @@
         <v>2</v>
       </c>
       <c r="C6" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -3217,10 +3208,10 @@
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -3234,10 +3225,10 @@
         <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -3251,10 +3242,10 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="E9">
         <v>2</v>
@@ -3268,10 +3259,10 @@
         <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="E10">
         <v>3</v>
@@ -3285,10 +3276,10 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -3302,10 +3293,10 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E12">
         <v>5</v>
@@ -3319,10 +3310,10 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="E13">
         <v>3</v>
@@ -3336,10 +3327,10 @@
         <v>4</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="E14">
         <v>4</v>
@@ -3353,7 +3344,7 @@
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -3367,10 +3358,10 @@
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="E16">
         <v>1</v>
@@ -3384,10 +3375,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -3416,13 +3407,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -3462,10 +3453,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3589,16 +3580,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3750,28 +3741,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:B83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.42578125" customWidth="1"/>
+    <col min="1" max="1" width="84.85546875" customWidth="1"/>
     <col min="2" max="2" width="37.140625" customWidth="1"/>
     <col min="3" max="64" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -3779,7 +3770,7 @@
         <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -3787,7 +3778,7 @@
         <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -3795,7 +3786,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -3803,7 +3794,7 @@
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -3811,343 +3802,343 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>39</v>
+        <v>337</v>
       </c>
       <c r="B8" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B11" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>57</v>
+        <v>348</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B16" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>66</v>
+        <v>338</v>
       </c>
       <c r="B17" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>72</v>
+        <v>339</v>
       </c>
       <c r="B19" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>78</v>
+        <v>340</v>
       </c>
       <c r="B21" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B23" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B24" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B25" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B26" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B28" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B30" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B31" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B32" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B33" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>330</v>
+        <v>341</v>
       </c>
       <c r="B34" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B35" t="s">
-        <v>332</v>
+        <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B36" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B37" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B38" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B39" t="s">
-        <v>334</v>
+        <v>322</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B40" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B41" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B42" t="s">
-        <v>335</v>
+        <v>323</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B43" t="s">
-        <v>336</v>
+        <v>324</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B44" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B45" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B46" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>156</v>
+        <v>342</v>
       </c>
       <c r="B47" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="B48" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="B49" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -4155,275 +4146,275 @@
         <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="B51" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B52" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="B53" t="s">
-        <v>338</v>
+        <v>326</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="B54" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="B55" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B57" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B58" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B59" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>193</v>
+        <v>343</v>
       </c>
       <c r="B60" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>196</v>
+        <v>344</v>
       </c>
       <c r="B61" t="s">
-        <v>339</v>
+        <v>327</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B62" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="B63" t="s">
-        <v>341</v>
+        <v>329</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="B64" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B65" t="s">
-        <v>333</v>
+        <v>321</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
       <c r="B66" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="8" t="s">
-        <v>212</v>
+        <v>345</v>
       </c>
       <c r="B67" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="B68" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B69" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="B70" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B71" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B72" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
-        <v>227</v>
+        <v>346</v>
       </c>
       <c r="B73" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="8" t="s">
-        <v>230</v>
+        <v>347</v>
       </c>
       <c r="B74" t="s">
-        <v>343</v>
+        <v>331</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
       <c r="B75" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B76" t="s">
-        <v>345</v>
+        <v>333</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B77" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="B78" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
       <c r="B79" t="s">
-        <v>346</v>
+        <v>334</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="B80" t="s">
-        <v>347</v>
+        <v>335</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="B81" t="s">
-        <v>340</v>
+        <v>328</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="B82" t="s">
-        <v>348</v>
+        <v>336</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="B83" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>